<commit_message>
added the recent newsblog, esricareer scripts
</commit_message>
<xml_diff>
--- a/data/EsriCareersMain_TC02.xlsx
+++ b/data/EsriCareersMain_TC02.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t>http://www.esri.com/careers/main</t>
   </si>
@@ -27,10 +27,97 @@
     <t>EsriCareersMainURL</t>
   </si>
   <si>
-    <t>We Are Esri</t>
-  </si>
-  <si>
     <t>careerMHdr</t>
+  </si>
+  <si>
+    <t>JDHdr</t>
+  </si>
+  <si>
+    <t>Inputdata</t>
+  </si>
+  <si>
+    <t>jobCategory</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>LHdr</t>
+  </si>
+  <si>
+    <t>REHeader</t>
+  </si>
+  <si>
+    <t>StuHdr</t>
+  </si>
+  <si>
+    <t>JCitemdata</t>
+  </si>
+  <si>
+    <t>LifeHdr</t>
+  </si>
+  <si>
+    <t>CHeader</t>
+  </si>
+  <si>
+    <t>BText</t>
+  </si>
+  <si>
+    <t>FName</t>
+  </si>
+  <si>
+    <t>LName</t>
+  </si>
+  <si>
+    <t>EmailID</t>
+  </si>
+  <si>
+    <t>PhoneNo</t>
+  </si>
+  <si>
+    <t>VConfNotific</t>
+  </si>
+  <si>
+    <t>JOB OPENINGS</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Information Technology</t>
+  </si>
+  <si>
+    <t>US-CA-Redlands</t>
+  </si>
+  <si>
+    <t>RECRUITING EVENTS</t>
+  </si>
+  <si>
+    <t>STUDENTS AT ESRI</t>
+  </si>
+  <si>
+    <t>Administrative Support</t>
+  </si>
+  <si>
+    <t>LIFE @ ESRI</t>
+  </si>
+  <si>
+    <t>CONTACT US</t>
+  </si>
+  <si>
+    <t>Test1</t>
+  </si>
+  <si>
+    <t>Ltest</t>
+  </si>
+  <si>
+    <t>balaji.harinath@htcindia.com</t>
+  </si>
+  <si>
+    <t>Thank You!</t>
+  </si>
+  <si>
+    <t>We Are Esri</t>
   </si>
 </sst>
 </file>
@@ -383,18 +470,21 @@
   <dimension ref="A1:Y2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="3" width="11.5703125"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125"/>
     <col min="4" max="4" width="9.5703125" customWidth="1"/>
     <col min="5" max="5" width="10.140625" customWidth="1"/>
     <col min="6" max="6" width="9.42578125" customWidth="1"/>
     <col min="7" max="7" width="11.5703125"/>
     <col min="8" max="8" width="8.28515625" customWidth="1"/>
-    <col min="9" max="24" width="11.5703125"/>
+    <col min="9" max="16" width="11.5703125"/>
+    <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
+    <col min="18" max="24" width="11.5703125"/>
     <col min="25" max="25" width="41.28515625" customWidth="1"/>
     <col min="26" max="1026" width="11.5703125"/>
   </cols>
@@ -404,34 +494,110 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="2"/>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
+        <v>32</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
+      <c r="G2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q2" s="4">
+        <v>44222222222</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>31</v>
+      </c>
       <c r="S2" s="4"/>
       <c r="T2" s="4"/>
       <c r="U2" s="4"/>
@@ -441,8 +607,11 @@
       <c r="Y2" s="5"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="P2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" r:id="rId1"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" r:id="rId2"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>